<commit_message>
Veranderingen doorgevoerd aan de hand van coachgesprek 3.
</commit_message>
<xml_diff>
--- a/Documentatie/Analyse/Database.xlsx
+++ b/Documentatie/Analyse/Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="29">
   <si>
     <t>MilanovDB v1:</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>typ_id</t>
+  </si>
+  <si>
+    <t>MilanovDB v3:</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Roles</t>
   </si>
 </sst>
 </file>
@@ -204,13 +216,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -252,13 +264,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -269,6 +281,102 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1581150" y="4514850"/>
+          <a:ext cx="1933575" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Rechte verbindingslijn met pijl 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="2609850"/>
+          <a:ext cx="762000" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Rechte verbindingslijn met pijl 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1581150" y="4133850"/>
           <a:ext cx="1933575" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -584,14 +692,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H29"/>
+  <dimension ref="A2:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -702,168 +811,317 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5" t="s">
+    <row r="18" spans="1:8">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="C19" s="4" t="s">
+      <c r="E18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
+    <row r="22" spans="1:8">
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="C23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="C27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="8"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="C33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="C35" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="3" t="s">
+    <row r="37" spans="2:8">
+      <c r="C37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="G37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="C23" s="4" t="s">
+    <row r="39" spans="2:8">
+      <c r="C39" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5" t="s">
+    <row r="40" spans="2:8">
+      <c r="B40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="C27" s="4" t="s">
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="C41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="C43" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
-      <c r="B28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    <row r="44" spans="2:8">
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="7"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="C45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>